<commit_message>
adicionado o arquivo 1.1 do relatorio principal
</commit_message>
<xml_diff>
--- a/Acessibilidade/relatorios/relatorio_principal_1.1.xlsx
+++ b/Acessibilidade/relatorios/relatorio_principal_1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2650831723019\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Legenda" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Relatorio!$A$1:$O$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Relatorio'!$A$1:$O$23</definedName>
     <definedName name="Gravidade">Legenda!$B$2:$B$4</definedName>
     <definedName name="Status">Legenda!$B$7:$B$10</definedName>
   </definedNames>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Atribuído</t>
   </si>
   <si>
-    <t>9/15/2018 19:00:00</t>
-  </si>
-  <si>
     <t>Usar o jQuery e com o evento "keypress ou keydown" desativar o redirecionamento</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>8/29/2018</t>
   </si>
   <si>
-    <t>9/15/2018 19:00</t>
-  </si>
-  <si>
     <t>Verificar permissão de arquivo no servidor</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>8/30/2018</t>
   </si>
   <si>
-    <t>9/16/2018 20:15</t>
-  </si>
-  <si>
     <t>Fazer ignorar o elemento desnecessario pelo tab</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>8/31/2018</t>
   </si>
   <si>
-    <t>9/17/2018 19:15</t>
-  </si>
-  <si>
     <t>Verificar se tem algo a ver com uma classe ou codigo js que foi colocado para fazer funcionar o clique de redirecionamento na tag “object”</t>
   </si>
   <si>
@@ -181,9 +169,6 @@
   </si>
   <si>
     <t>É possivel dar o checked pela tacla space</t>
-  </si>
-  <si>
-    <t>9/15/2018 20:00:00</t>
   </si>
   <si>
     <t>Jéssica</t>
@@ -825,7 +810,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Cambria"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -901,101 +937,6 @@
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEFA34F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6A5FFB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Cambria"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1323,10 +1264,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3000,14 +2941,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="relatorio" displayName="relatorio" ref="A1:O1048576" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="relatorio" displayName="relatorio" ref="A1:O1048576" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:O1048576"/>
   <tableColumns count="15">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Persona"/>
     <tableColumn id="3" name="Software"/>
     <tableColumn id="4" name="Erro"/>
-    <tableColumn id="5" name="Url" dataDxfId="11"/>
+    <tableColumn id="5" name="Url" dataDxfId="0"/>
     <tableColumn id="6" name="Gravidade"/>
     <tableColumn id="7" name="Descrição"/>
     <tableColumn id="8" name="Ação corretiva"/>
@@ -3322,8 +3263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3335,7 +3276,7 @@
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.5703125" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1"/>
+    <col min="8" max="8" width="71.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="11" width="16.7109375" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
@@ -3427,14 +3368,14 @@
       <c r="K2" s="16">
         <v>43374</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19">
+        <v>43358</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="N2" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O2" s="17"/>
       <c r="P2" s="22"/>
@@ -3449,38 +3390,38 @@
         <v>15</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="16">
         <v>43374</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="19">
+        <v>43358</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="23"/>
@@ -3498,35 +3439,35 @@
         <v>16</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="G4" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K4" s="16">
         <v>43374</v>
       </c>
-      <c r="L4" s="17" t="s">
-        <v>38</v>
+      <c r="L4" s="19">
+        <v>43359</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O4" s="17"/>
       <c r="P4" s="22"/>
@@ -3544,35 +3485,35 @@
         <v>16</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K5" s="16">
         <v>43374</v>
       </c>
-      <c r="L5" s="20" t="s">
-        <v>45</v>
+      <c r="L5" s="19">
+        <v>43360</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="22"/>
@@ -3590,19 +3531,19 @@
         <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>21</v>
@@ -3613,14 +3554,14 @@
       <c r="K6" s="16">
         <v>43374</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>50</v>
+      <c r="L6" s="19">
+        <v>43358</v>
       </c>
       <c r="M6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="22"/>
@@ -3632,25 +3573,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>21</v>
@@ -3661,10 +3602,10 @@
       <c r="K7" s="16">
         <v>43374</v>
       </c>
-      <c r="L7" s="20"/>
+      <c r="L7" s="19"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="22"/>
@@ -3676,28 +3617,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="J8" s="16">
         <v>43341</v>
@@ -3705,14 +3646,18 @@
       <c r="K8" s="16">
         <v>43374</v>
       </c>
-      <c r="L8" s="17"/>
+      <c r="L8" s="19">
+        <v>43376</v>
+      </c>
       <c r="M8" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="O8" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
@@ -3722,28 +3667,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="J9" s="19">
         <v>43342</v>
@@ -3751,12 +3696,16 @@
       <c r="K9" s="19">
         <v>43374</v>
       </c>
-      <c r="L9" s="20"/>
+      <c r="L9" s="19">
+        <v>43376</v>
+      </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O9" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="P9" s="23"/>
       <c r="Q9" s="23"/>
       <c r="R9" s="23"/>
@@ -3766,28 +3715,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="J10" s="16">
         <v>43343</v>
@@ -3795,12 +3744,16 @@
       <c r="K10" s="16">
         <v>43374</v>
       </c>
-      <c r="L10" s="17"/>
+      <c r="L10" s="19">
+        <v>43376</v>
+      </c>
       <c r="M10" s="10"/>
       <c r="N10" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="O10" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
@@ -3810,13 +3763,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>18</v>
@@ -3825,10 +3778,10 @@
         <v>19</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>21</v>
@@ -3839,10 +3792,10 @@
       <c r="K11" s="16">
         <v>43375</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="19"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O11" s="10"/>
       <c r="P11" s="22"/>
@@ -3854,25 +3807,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>21</v>
@@ -3885,10 +3838,10 @@
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="22"/>
@@ -3900,39 +3853,39 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>78</v>
-      </c>
       <c r="H13" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="22"/>
@@ -3944,39 +3897,39 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="10"/>
       <c r="N14" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="22"/>
@@ -3988,39 +3941,39 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L15" s="20"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="23"/>
@@ -4032,39 +3985,39 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L16" s="17"/>
       <c r="M16" s="10"/>
       <c r="N16" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O16" s="17"/>
       <c r="P16" s="22"/>
@@ -4076,39 +4029,39 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L17" s="20"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O17" s="10"/>
       <c r="P17" s="22"/>
@@ -4120,25 +4073,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>21</v>
@@ -4152,7 +4105,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="10"/>
       <c r="N18" s="17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O18" s="17"/>
       <c r="P18" s="22"/>
@@ -4164,31 +4117,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K19" s="19">
         <v>43393</v>
@@ -4196,7 +4149,7 @@
       <c r="L19" s="20"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O19" s="10"/>
       <c r="P19" s="23"/>
@@ -4208,31 +4161,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K20" s="16">
         <v>43393</v>
@@ -4240,7 +4193,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="10"/>
       <c r="N20" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O20" s="17"/>
       <c r="P20" s="22"/>
@@ -4252,31 +4205,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K21" s="19">
         <v>43393</v>
@@ -4284,7 +4237,7 @@
       <c r="L21" s="20"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O21" s="10"/>
       <c r="P21" s="22"/>
@@ -4296,31 +4249,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K22" s="16">
         <v>43393</v>
@@ -4328,7 +4281,7 @@
       <c r="L22" s="17"/>
       <c r="M22" s="10"/>
       <c r="N22" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O22" s="17"/>
       <c r="P22" s="23"/>
@@ -4340,31 +4293,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K23" s="19">
         <v>43393</v>
@@ -4372,7 +4325,7 @@
       <c r="L23" s="20"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O23" s="10"/>
       <c r="P23" s="23"/>
@@ -4384,31 +4337,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K24" s="16">
         <v>43393</v>
@@ -4416,7 +4369,7 @@
       <c r="L24" s="17"/>
       <c r="M24" s="10"/>
       <c r="N24" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O24" s="17"/>
     </row>
@@ -4425,31 +4378,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K25" s="19">
         <v>43393</v>
@@ -4457,7 +4410,7 @@
       <c r="L25" s="20"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O25" s="10"/>
     </row>
@@ -4466,31 +4419,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="F26" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K26" s="16">
         <v>43393</v>
@@ -4498,7 +4451,7 @@
       <c r="L26" s="17"/>
       <c r="M26" s="10"/>
       <c r="N26" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="O26" s="17"/>
     </row>
@@ -4507,25 +4460,25 @@
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>21</v>
@@ -4539,7 +4492,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O27" s="10"/>
     </row>
@@ -4548,25 +4501,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>21</v>
@@ -4580,7 +4533,7 @@
       <c r="L28" s="17"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O28" s="17"/>
     </row>
@@ -4589,25 +4542,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C29" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="E29" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>21</v>
@@ -4621,7 +4574,7 @@
       <c r="L29" s="20"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="O29" s="10"/>
     </row>
@@ -4630,25 +4583,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>21</v>
@@ -4662,7 +4615,7 @@
       <c r="L30" s="17"/>
       <c r="M30" s="10"/>
       <c r="N30" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O30" s="17"/>
     </row>
@@ -4671,25 +4624,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>156</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>21</v>
@@ -4703,7 +4656,7 @@
       <c r="L31" s="20"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O31" s="10"/>
     </row>
@@ -4712,25 +4665,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>21</v>
@@ -4744,7 +4697,7 @@
       <c r="L32" s="37"/>
       <c r="M32" s="37"/>
       <c r="N32" s="37" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O32" s="37"/>
     </row>
@@ -4753,25 +4706,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>19</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H33" s="37" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>21</v>
@@ -4785,7 +4738,7 @@
       <c r="L33" s="37"/>
       <c r="M33" s="37"/>
       <c r="N33" s="37" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O33" s="37"/>
     </row>
@@ -4794,25 +4747,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>21</v>
@@ -4826,7 +4779,7 @@
       <c r="L34" s="17"/>
       <c r="M34" s="10"/>
       <c r="N34" s="37" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="O34" s="17"/>
     </row>
@@ -5360,27 +5313,27 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Leve"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"Moderado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Crítico"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Sem ação"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Atribuído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Não Atribuído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Corrigido"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5421,31 +5374,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F1" s="33" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B2" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Corrigido")</f>
-        <v>0</v>
+        <f>COUNTIF('Relatorio'!I2:I65,"Corrigido")</f>
+        <v>3</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Crítico")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Crítico")</f>
         <v>10</v>
       </c>
     </row>
@@ -5454,39 +5407,39 @@
         <v>21</v>
       </c>
       <c r="B3" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Atribuído")</f>
-        <v>33</v>
+        <f>COUNTIF('Relatorio'!I2:I65,"Atribuído")</f>
+        <v>30</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G3" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Moderado")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Moderado")</f>
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B4" s="26">
-        <f>COUNTIF(Relatorio!I2:I65,"Não Atribuído")</f>
+        <f>COUNTIF('Relatorio'!I2:I65,"Não Atribuído")</f>
         <v>0</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" s="26">
-        <f>COUNTIF(Relatorio!F2:F65,"Leve")</f>
+        <f>COUNTIF('Relatorio'!F2:F65,"Leve")</f>
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B5" s="26">
-        <f>COUNTIF(Relatorio!I5:I68,"Sem Ação")</f>
+        <f>COUNTIF('Relatorio'!I5:I68,"Sem Ação")</f>
         <v>0</v>
       </c>
     </row>
@@ -5524,25 +5477,25 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -5552,10 +5505,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -5563,23 +5516,23 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>